<commit_message>
I did this commit because im going to add one function in the next versions
</commit_message>
<xml_diff>
--- a/Sustantivos_Aleman_Completo.xlsx
+++ b/Sustantivos_Aleman_Completo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="158" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
@@ -336,8 +336,8 @@
   </sheetPr>
   <dimension ref="A1:F298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="D287" sqref="D287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="0"/>
@@ -346,7 +346,7 @@
     <col width="24.140625" customWidth="1" min="2" max="2"/>
     <col width="38.85546875" customWidth="1" min="3" max="3"/>
     <col width="98.28515625" customWidth="1" min="4" max="4"/>
-    <col width="59.7109375" customWidth="1" min="5" max="5"/>
+    <col width="142.140625" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1255,6 +1255,12 @@
           <t>Der Lebenslauf ist, ebenso wie die Zeugnisse und die Berufserfahrung, sehr wichtig für eine Bewerbung</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El currículum, así como los certificados y la experiencia profesional, son muy importantes para una solicitud.</t>
+        </is>
+      </c>
       <c r="F27" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1283,6 +1289,12 @@
           <t>Im Lebenslauf solltest du auch deine berufliche Erfahrung eintragen</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+En el currículum también deberías incluir tu experiencia profesional.</t>
+        </is>
+      </c>
       <c r="F28" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1311,6 +1323,12 @@
           <t>Persönliche Fähigkeiten sind zum Beispiel Intelligenz oder Ernsthaftigkeit.</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Las habilidades personales son, por ejemplo, la inteligencia o la seriedad.</t>
+        </is>
+      </c>
       <c r="F29" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1339,6 +1357,12 @@
           <t>Im Lebenslauf sollte man persönliche Daten, die Berufserfahrung, die Ausbildung, aber auch die persönlichen Fähigkeiten angeben.</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+En el curriculum vitae, se debe indicar los datos personales, la experiencia laboral, la formación, así como las habilidades personales.</t>
+        </is>
+      </c>
       <c r="F30" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1367,6 +1391,12 @@
           <t>Der Befrager ist im Allgemeinen ein Mitarbeiter der Personalabteilung.</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El encuestador generalmente es un empleado de la oficina de Personal.</t>
+        </is>
+      </c>
       <c r="F31" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1395,6 +1425,12 @@
           <t>aber Schwächen habe ich mit Sicherheit keine!</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Pero, ¡con seguridad no tengo ninguna debilidad!</t>
+        </is>
+      </c>
       <c r="F32" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1424,6 +1460,12 @@
 Ich möchte gerne an dieser Stelle ein Bild machen.</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Querría tomar una foto en este lugar.</t>
+        </is>
+      </c>
       <c r="F33" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1452,6 +1494,12 @@
           <t>Um eine neue Arbeitsstelle zu finden, sollte man einige Stellenanzeigen durchlesen.</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Para encontrar un nuevo empleo, debería leer algunos anuncios de empleo.</t>
+        </is>
+      </c>
       <c r="F34" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1480,6 +1528,12 @@
           <t>Der Geschäftsführer leitet das gesamte Unternehmen und hat eine große Verantwortung.</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El gerente dirige toda la empresa y tiene una gran responsabilidad.</t>
+        </is>
+      </c>
       <c r="F35" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1508,6 +1562,12 @@
           <t>Der Lebenslauf ist, ebenso wie die Zeugnisse und die Berufserfahrung, sehr wichtig für eine Bewerbung</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El currículum, al igual que los certificados y la experiencia laboral, es muy importante para una solicitud.</t>
+        </is>
+      </c>
       <c r="F36" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1536,6 +1596,12 @@
           <t>Das Anschreiben begleitet den Lebenslauf und stellt eine wichtige Bewerbungsunterlage dar</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El currículum vitae va acompañado de la carta de presentación que es un documento clave en la solicitud de empleo.</t>
+        </is>
+      </c>
       <c r="F37" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1564,6 +1630,12 @@
           <t>Meine Stärken und Schwächen? Ich kann gut Deutsch sprechen und habe viel Erfahrung</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> mit Computern.
+Mis fortalezas y debilidades? Puedo hablar alemán bien y tengo mucha experiencia con computadoras.</t>
+        </is>
+      </c>
       <c r="F38" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1592,6 +1664,12 @@
           <t>Der Befrager ist im Allgemeinen ein Mitarbeiter der Personalabteilung.</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El entrevistador generalmente es un empleado del departamento de recursos humanos.</t>
+        </is>
+      </c>
       <c r="F39" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1620,6 +1698,12 @@
           <t>dass zum Beispiel dein Online-Shop das beste Angebot im ganzen Internet hat</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Que por ejemplo, tu tienda en línea tenga la mejor oferta en toda la Internet.</t>
+        </is>
+      </c>
       <c r="F40" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1648,6 +1732,12 @@
           <t>Oder Bauwesen? Nicht schlecht</t>
         </is>
       </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+¿Arquitectura o Ingeniería? ¡No está mal!</t>
+        </is>
+      </c>
       <c r="F41" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1676,6 +1766,12 @@
           <t>Nicht zuletzt muss er seine Ergebnisse der Geschäftsführung mitteilen</t>
         </is>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>.
+Último pero no menos importante, debe comunicar sus resultados al consejo de administración.</t>
+        </is>
+      </c>
       <c r="F42" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1704,6 +1800,12 @@
           <t>Das Hauptziel eines Online-Marketing-Managers ist meistens</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> es, das Markenbild eines Unternehmens aufzubauen.
+El principal objetivo de un gerente de marketing en línea suele ser construir la imagen de marca de una empresa.</t>
+        </is>
+      </c>
       <c r="F43" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1732,6 +1834,12 @@
           <t>Für jede neue Arbeitsstelle muss man einen Arbeitsvertrag unterzeichnen</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Para cada nuevo trabajo, se debe firmar un contrato de trabajo.</t>
+        </is>
+      </c>
       <c r="F44" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1760,6 +1868,12 @@
           <t>Er braucht Teamgeist, denn die Kommunikation mit anderen Abteilungen und Bereichen des Unternehmens ist sehr wichtig</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Él necesita espíritu de equipo, ya que la comunicación con otros departamentos y áreas de la empresa es muy importante.</t>
+        </is>
+      </c>
       <c r="F45" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1783,6 +1897,18 @@
 Der Berufsberater → Die Berufsberater</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Berufsberater kann dabei hilfreich sein, eine berufliche Richtung einzuschlagen, die zu den eigenen Interessen und Fähigkeiten passt.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El asesor profesional puede ser de ayuda para elegir una dirección profesional que se adapte a los intereses y habilidades propios.</t>
+        </is>
+      </c>
       <c r="F46" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1800,10 +1926,21 @@
           <t>der Erfolg</t>
         </is>
       </c>
-      <c r="C47" s="1" t="n"/>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Erfolge.</t>
+        </is>
+      </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
           <t>denn nur so kann er sein Ziel erreichen und Erfolg auf dem Markt haben.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Porque solo de esta manera podrá alcanzar su objetivo y tener éxito en el mercado.</t>
         </is>
       </c>
       <c r="F47" s="1" t="inlineStr">
@@ -1834,6 +1971,12 @@
           <t>Sein Tagesablauf ist nicht Routine</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Su rutina diaria no es rutinaria.</t>
+        </is>
+      </c>
       <c r="F48" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1862,6 +2005,12 @@
           <t>Er braucht Teamgeist, denn die Kommunikation mit anderen Abteilungen und Bereichen des Unternehmens ist sehr wichtig</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>.
+Él necesita espíritu de equipo, ya que la comunicación con otros departamentos y áreas de la empresa es muy importante.</t>
+        </is>
+      </c>
       <c r="F49" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1890,6 +2039,12 @@
           <t>Kann einen komplexen Text über neue Berufe verstehen</t>
         </is>
       </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Puede entender un texto complejo sobre nuevos oficios.</t>
+        </is>
+      </c>
       <c r="F50" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1918,6 +2073,12 @@
           <t>Er braucht Teamgeist, denn die Kommunikation mit anderen Abteilungen und Bereichen des Unternehmens ist sehr wichtig</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Él necesita espíritu de equipo, ya que la comunicación con otros departamentos y áreas de la empresa es muy importante.</t>
+        </is>
+      </c>
       <c r="F51" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1946,6 +2107,12 @@
           <t>aber auch hier gibt es schon so viele Programme und Anwendungen</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Pero también hay muchos programas y aplicaciones aquí.</t>
+        </is>
+      </c>
       <c r="F52" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1969,6 +2136,18 @@
 die Berufsberatungen</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Berufsberatung kann helfen, den richtigen Beruf für mich zu finden.</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La orientación profesional puede ayudar a encontrar el trabajo adecuado para mí.</t>
+        </is>
+      </c>
       <c r="F53" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -1992,6 +2171,18 @@
 die Fortbildungen</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich nehme an der Fortbildung teil, um mein Wissen aufzufrischen.</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tomo la formación para refrescar mis conocimientos.</t>
+        </is>
+      </c>
       <c r="F54" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2020,6 +2211,12 @@
           <t>denn diese Programmiersprachen entwickeln sich mit einer unglaublichen Geschwindigkeit</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Porque estos lenguajes de programación están evolucionando a una velocidad increíble.</t>
+        </is>
+      </c>
       <c r="F55" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2048,6 +2245,12 @@
           <t>Du hast gerade deine Reifeprüfung abgelegt und stehst vor einer großen Herausforderung</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Acabas de terminar tu examen de madurez y te enfrentas a un gran reto.</t>
+        </is>
+      </c>
       <c r="F56" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2076,6 +2279,12 @@
           <t>Du hast gerade deine Reifeprüfung abgelegt</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Acabas de pasar tu examen de madurez.</t>
+        </is>
+      </c>
       <c r="F57" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2104,6 +2313,12 @@
           <t>dann mit einer Weiterbildung und nicht zuletzt mit einem Praktikum</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Entonces con una formación continua y no menos importante con una práctica.</t>
+        </is>
+      </c>
       <c r="F58" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2132,6 +2347,12 @@
           <t>Nicht zuletzt muss er genau wissen, welche die Zielgruppe ist,</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+No por ultimo, él debe saber exactamente quién es el público objetivo.</t>
+        </is>
+      </c>
       <c r="F59" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2160,6 +2381,12 @@
           <t>Nicht zuletzt muss er seine Ergebnisse der Geschäftsführung mitteilen</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>.
+No menos importante, debe notificar los resultados a la gerencia.</t>
+        </is>
+      </c>
       <c r="F60" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2183,6 +2410,18 @@
 Der Berufswege</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mein beruflicher Weg hat mich in die verschiedensten Richtungen geführt.</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mi camino profesional me ha llevado por diferentes direcciones.</t>
+        </is>
+      </c>
       <c r="F61" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2206,6 +2445,18 @@
 Die Seefahrer.</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Seefahrer konnte die bedrohliche Küste schnell erreichen.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El navegante pudo llegar rápidamente a la costa amenazadora.</t>
+        </is>
+      </c>
       <c r="F62" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2229,6 +2480,18 @@
 Die Teamgeister</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Teamgeist ist eine wichtige Komponente, um erfolgreich zusammenzuarbeiten.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El espíritu de equipo es un componente importante para trabajar con éxito en conjunto.</t>
+        </is>
+      </c>
       <c r="F63" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2252,6 +2515,18 @@
 Die Wissenschaftler.</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Wissenschaftler hat bereits viele Jahre an seiner Forschungsarbeit gearbeitet.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El científico ha estado trabajando en su investigación por muchos años.</t>
+        </is>
+      </c>
       <c r="F64" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2275,6 +2550,18 @@
 die Ausstrahlungen</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Sie hatte eine sehr angenehme Ausstrahlung.</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ella tenía una presencia muy agradable.</t>
+        </is>
+      </c>
       <c r="F65" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2298,6 +2585,18 @@
 die Behinderungen</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Behinderung ist in vielerlei Hinsicht ein Hindernis für Menschen.</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La discapacidad es un obstáculo para las personas de muchas maneras.</t>
+        </is>
+      </c>
       <c r="F66" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2321,6 +2620,18 @@
 die Regelmäßigkeiten</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich schätze die Regelmäßigkeit meiner täglichen Morgenroutine.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Valoro la regularidad de mi rutina diaria de la mañana.</t>
+        </is>
+      </c>
       <c r="F67" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2344,6 +2655,18 @@
 Die Werkstätten</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+In der Werkstatt werden Reparaturen an Autos und anderen Geräten durchgeführt.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+En el taller se realizan reparaciones de autos y otros equipos.</t>
+        </is>
+      </c>
       <c r="F68" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2367,6 +2690,18 @@
 Die Flüge</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Flug in die Ferien war eine willkommene Abwechslung.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El vuelo a las vacaciones fue una bienvenida variación.</t>
+        </is>
+      </c>
       <c r="F69" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2390,6 +2725,18 @@
 Die Flughäfen</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Flughafen ist der zweitgrößte internationale Verkehrsknotenpunkt der Stadt.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El aeropuerto es el segundo punto de tráfico internacional más grande de la ciudad.</t>
+        </is>
+      </c>
       <c r="F70" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2418,6 +2765,12 @@
           <t>eine Leiche im Keller</t>
         </is>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Una cadáver en el sótano.</t>
+        </is>
+      </c>
       <c r="F71" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2446,6 +2799,12 @@
           <t>einen Mangel beseitigen</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Eliminar una carencia.</t>
+        </is>
+      </c>
       <c r="F72" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2474,6 +2833,12 @@
           <t>was ist der Unterschied zwischen Ding und Sache?</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+¿Cuál es la diferencia entre "cosa" y "cosas"?</t>
+        </is>
+      </c>
       <c r="F73" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2502,6 +2867,12 @@
           <t>ich ziehe mir die Stiefel aus</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Me estoy quitando los botines.</t>
+        </is>
+      </c>
       <c r="F74" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2530,6 +2901,12 @@
           <t>die Wahrscheinlichkeit, dass wir uns sehen ist sehr groß</t>
         </is>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La probabilidad de vernos es muy grande.</t>
+        </is>
+      </c>
       <c r="F75" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2553,6 +2930,18 @@
 die Wiederholungen</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Wiederholung ist essentiell, um etwas wirklich zu lernen.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La repetición es esencial para realmente aprender algo.</t>
+        </is>
+      </c>
       <c r="F76" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2576,6 +2965,18 @@
 die Flugzeuge</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Flugzeug ist eines der schnellsten Verkehrsmittel.</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El avión es uno de los medios de transporte más rápidos.</t>
+        </is>
+      </c>
       <c r="F77" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2599,6 +3000,18 @@
 Die Treiben.</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Treiben auf dem Marktplatz war ein einziges Gewimmel.</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El bullicio en la plaza del mercado era una auténtica algarabía.</t>
+        </is>
+      </c>
       <c r="F78" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2627,6 +3040,12 @@
           <t>vor jdm/etw (dat) Angst haben</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tener miedo de alguien/algo.</t>
+        </is>
+      </c>
       <c r="F79" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2645,6 +3064,18 @@
         </is>
       </c>
       <c r="C80" s="1" t="n"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Ansehen, das er sich erarbeitet hat, ist beeindruckend.</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El respeto que se ha ganado es impresionante.</t>
+        </is>
+      </c>
       <c r="F80" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2668,6 +3099,18 @@
 die Aufrichtigkeiten</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich schätze die Aufrichtigkeit in einer Beziehung sehr.</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Valoro mucho la sinceridad en una relación.</t>
+        </is>
+      </c>
       <c r="F81" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2691,6 +3134,18 @@
 Die Decken.</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich habe mich unter die Decke gekuschelt.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Me acurruqué debajo de la manta.</t>
+        </is>
+      </c>
       <c r="F82" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2714,6 +3169,18 @@
 die Möglichkeiten</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>en
+Wir müssen die Möglichkeiten nutzen, um unser Ziel zu erreichen.</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tenemos que usar las posibilidades para alcanzar nuestro objetivo.</t>
+        </is>
+      </c>
       <c r="F83" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2737,6 +3204,18 @@
 die Schlangen</t>
         </is>
       </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Schlange kroch langsam durch das hohe Gras.</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La serpiente se arrastró lentamente a través de la alta hierba.</t>
+        </is>
+      </c>
       <c r="F84" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2765,6 +3244,12 @@
           <t>jdm Schuld geben / es war meine Schuld</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Le di culpa a alguien / fue mi culpa.</t>
+        </is>
+      </c>
       <c r="F85" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2788,6 +3273,18 @@
 die Wahln</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich bin mir bewusst, dass die Wahl entscheidend für meine Zukunft sein kann.</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Soy consciente de que mi elección puede ser determinante para mi futuro.</t>
+        </is>
+      </c>
       <c r="F86" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2816,6 +3313,12 @@
           <t>eine Umdrehung des Lenkrades</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Una vuelta de la rueda de dirección.</t>
+        </is>
+      </c>
       <c r="F87" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2844,6 +3347,12 @@
           <t>ganz im gegenteil</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Todo lo contrario</t>
+        </is>
+      </c>
       <c r="F88" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2867,6 +3376,18 @@
 Die Berufe.</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mein Traumberuf ist der Beruf eines Lehrers.</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mi profesión de sueño es ser maestro.</t>
+        </is>
+      </c>
       <c r="F89" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2890,6 +3411,18 @@
 Die Personen</t>
         </is>
       </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Person ist sehr nett.</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La persona es muy amable.</t>
+        </is>
+      </c>
       <c r="F90" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2907,7 +3440,24 @@
           <t>die Personen</t>
         </is>
       </c>
-      <c r="C91" s="1" t="n"/>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Personen.</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mehrere Personen kamen zur Party.</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Varios personas vinieron a la fiesta.</t>
+        </is>
+      </c>
       <c r="F91" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2931,6 +3481,18 @@
 die Leute</t>
         </is>
       </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Leute freuen sich über das schöne Wetter.</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+La gente se alegra por el buen tiempo.</t>
+        </is>
+      </c>
       <c r="F92" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2954,6 +3516,18 @@
 die Tätigkeiten</t>
         </is>
       </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich genieße die Tätigkeit, die ich jeden Tag ausübe.</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Disfruto la actividad que realizo todos los días.</t>
+        </is>
+      </c>
       <c r="F93" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -2977,6 +3551,18 @@
 Die Nachbarn</t>
         </is>
       </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Nachbar hat heute früh vor unserer Tür gestanden.</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El vecino estaba parado afuera de nuestra puerta esta mañana.</t>
+        </is>
+      </c>
       <c r="F94" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3000,6 +3586,18 @@
 Die Heimatländer</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Heimatland ist die Heimat für viele Menschen.</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El país de origen es el hogar para muchas personas.</t>
+        </is>
+      </c>
       <c r="F95" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3023,6 +3621,18 @@
 Die Wohnorte.</t>
         </is>
       </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Wohnort meiner Familie ist in Bayern.</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El lugar de residencia de mi familia está en Baviera.</t>
+        </is>
+      </c>
       <c r="F96" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3046,6 +3656,18 @@
 Die Geburtsorte.</t>
         </is>
       </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Geburtsort meiner Eltern ist Deutschland.</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El lugar de nacimiento de mis padres es Alemania.</t>
+        </is>
+      </c>
       <c r="F97" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3069,6 +3691,18 @@
 Die Studien.</t>
         </is>
       </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich gehe demnächst ins Ausland, um das Studium zu beginnen.</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Yo voy a salir pronto al extranjero para comenzar mis estudios.</t>
+        </is>
+      </c>
       <c r="F98" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3092,6 +3726,18 @@
 Die Diplomen</t>
         </is>
       </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>.
+Nach ihrem Studium hat sie ihr Diplom in der Tasche.</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Después de sus estudios, ella tiene su diploma en su bolsillo.</t>
+        </is>
+      </c>
       <c r="F99" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3115,6 +3761,18 @@
 Die Prüfer.</t>
         </is>
       </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Prüfer wird heute alle Prüfungsergebnisse bekannt geben.</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El evaluador dará a conocer todos los resultados de la prueba hoy.</t>
+        </is>
+      </c>
       <c r="F100" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3138,6 +3796,18 @@
 Die Briefe</t>
         </is>
       </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Brief ist schon vor einigen Tagen angekommen.</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El carta llegó hace algunos días.</t>
+        </is>
+      </c>
       <c r="F101" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3161,6 +3831,18 @@
 die Bewerbungen</t>
         </is>
       </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich habe die Bewerbung bereits ausgefüllt und abgeschickt.</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ya he rellenado la solicitud y la he enviado.</t>
+        </is>
+      </c>
       <c r="F102" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3184,6 +3866,18 @@
 Die Bescheide.</t>
         </is>
       </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Bescheid wurde heute erhalten.</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El aviso fue recibido hoy.</t>
+        </is>
+      </c>
       <c r="F103" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3207,6 +3901,18 @@
 die Mitteilungen, die Bescheide</t>
         </is>
       </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Mitteilung, der mir heute zugeschickt wurde, gibt mir den endgültigen Bescheid.</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La comunicación que me enviaron hoy me da la respuesta definitiva.</t>
+        </is>
+      </c>
       <c r="F104" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3230,6 +3936,18 @@
 die Beratungen</t>
         </is>
       </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+„Ich freue mich auf die Beratung morgen.“</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Me entusiasmo con la consulta mañana.</t>
+        </is>
+      </c>
       <c r="F105" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3247,7 +3965,24 @@
           <t>die Miete</t>
         </is>
       </c>
-      <c r="C106" s="1" t="n"/>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Mieten</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Miete muss bei unserem Vermieter jeden Monat pünktlich bezahlt werden.</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La renta debe ser pagada puntualmente a nuestro arrendador cada mes.</t>
+        </is>
+      </c>
       <c r="F106" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3271,6 +4006,18 @@
 die Freizeiten</t>
         </is>
       </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+In meiner Freizeit gehe ich gerne mit Freunden spazieren.</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+En mi tiempo libre me gusta salir de paseo con mis amigos.</t>
+        </is>
+      </c>
       <c r="F107" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3294,6 +4041,18 @@
 die Dinge</t>
         </is>
       </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Ding sieht seltsam aus.</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Esa cosa se ve extraña.</t>
+        </is>
+      </c>
       <c r="F108" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3317,6 +4076,18 @@
 Die Lösungen</t>
         </is>
       </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Lösung ist Teil des Problems und muss daher gefunden werden.</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La solución es parte del problema y por lo tanto debe ser encontrada.</t>
+        </is>
+      </c>
       <c r="F109" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3335,6 +4106,18 @@
         </is>
       </c>
       <c r="C110" s="1" t="n"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Lösungen für dieses Problem sind schwer zu finden.</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Las soluciones para este problema son difíciles de encontrar.</t>
+        </is>
+      </c>
       <c r="F110" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3358,6 +4141,18 @@
 die Termine</t>
         </is>
       </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Termin war wichtig, um zu besprechen, was als nächstes zu tun ist.</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El encuentro era importante para discutir qué hacer a continuación.</t>
+        </is>
+      </c>
       <c r="F111" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3381,6 +4176,18 @@
 die Kunden</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Kunde hat sich schnell verbreitet.</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La noticia se propagó rápidamente.</t>
+        </is>
+      </c>
       <c r="F112" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3404,6 +4211,18 @@
 Die Sekretariate</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Sekretariat ist der Ort, an dem man am besten Informationen über die Universität erhalten kann.</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El Secretariado es el lugar ideal para obtener información sobre la universidad.</t>
+        </is>
+      </c>
       <c r="F113" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3427,6 +4246,18 @@
 Die Informatiker</t>
         </is>
       </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Informatiker hat ein breites Wissen in vielen Bereichen der Technik.</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El informático tiene un amplio conocimiento en muchas áreas de la tecnología.</t>
+        </is>
+      </c>
       <c r="F114" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -3444,7 +4275,24 @@
           <t>der Koch</t>
         </is>
       </c>
-      <c r="C115" s="1" t="n"/>
+      <c r="C115" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Köche</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Koch machte ein feines Abendessen für die Gäste.</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El cocinero hizo una deliciosa cena para los invitados.</t>
+        </is>
+      </c>
       <c r="F115" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -7225,20 +8073,12 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>la ragazza</t>
-        </is>
-      </c>
-      <c r="B298" s="1" t="inlineStr">
-        <is>
-          <t>Lei è una ragazza intelligente</t>
-        </is>
-      </c>
+          <t>der Anfang</t>
+        </is>
+      </c>
+      <c r="B298" s="1" t="n"/>
       <c r="C298" s="1" t="n"/>
-      <c r="D298" s="1" t="inlineStr">
-        <is>
-          <t>la chica</t>
-        </is>
-      </c>
+      <c r="D298" s="1" t="n"/>
       <c r="F298" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>

</xml_diff>

<commit_message>
Preparation before posting the project in github
</commit_message>
<xml_diff>
--- a/Sustantivos_Aleman_Completo.xlsx
+++ b/Sustantivos_Aleman_Completo.xlsx
@@ -3063,7 +3063,12 @@
           <t>die Ansehen</t>
         </is>
       </c>
-      <c r="C80" s="1" t="n"/>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>:
+die Ansehenen</t>
+        </is>
+      </c>
       <c r="D80" t="inlineStr">
         <is>
           <t xml:space="preserve">
@@ -4310,7 +4315,24 @@
           <t>der/die Kellner/rin</t>
         </is>
       </c>
-      <c r="C116" s="1" t="n"/>
+      <c r="C116" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Kellner/innen</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Kellner brachte uns die bestellten Getränke.</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El mesero nos trajo las bebidas pedidas.</t>
+        </is>
+      </c>
       <c r="F116" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4328,7 +4350,24 @@
           <t>der Arzt</t>
         </is>
       </c>
-      <c r="C117" s="1" t="n"/>
+      <c r="C117" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Ärzte</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Arzt wird mir helfen, meine Beschwerden zu lindern.</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El médico me ayudará a aliviar mis molestias.</t>
+        </is>
+      </c>
       <c r="F117" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4346,7 +4385,24 @@
           <t>der Unterricht</t>
         </is>
       </c>
-      <c r="C118" s="1" t="n"/>
+      <c r="C118" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Unterrichte sind die Plurale der Unterricht.</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Unterricht ist heute sehr interessant.</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La clase es muy interesante hoy.</t>
+        </is>
+      </c>
       <c r="F118" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4365,9 +4421,21 @@
 Die Schöpfung</t>
         </is>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Schöpfungen</t>
+        </is>
+      </c>
       <c r="D119" s="1" t="inlineStr">
         <is>
           <t>die Bildung</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La educación</t>
         </is>
       </c>
       <c r="F119" s="1" t="inlineStr">
@@ -4387,7 +4455,24 @@
           <t>die Vergangenheit</t>
         </is>
       </c>
-      <c r="C120" s="1" t="n"/>
+      <c r="C120" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Vergangenheiten</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Vergangenheit hat uns gelehrt, wie wir uns verbessern können.</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La historia nos ha enseñado cómo podemos mejorar.</t>
+        </is>
+      </c>
       <c r="F120" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4405,7 +4490,24 @@
           <t>die Verwendung</t>
         </is>
       </c>
-      <c r="C121" s="1" t="n"/>
+      <c r="C121" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> und seiner Flexion
+die Verwendungen</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Verwendung dieser Technologie ist sehr einfach.</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El uso de esta tecnología es muy sencillo.</t>
+        </is>
+      </c>
       <c r="F121" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4424,9 +4526,21 @@
 Der Weihnachtsgesang</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Weihnachtsgesänge</t>
+        </is>
+      </c>
       <c r="D122" s="1" t="inlineStr">
         <is>
           <t>das Weihnachtslied</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La canción de Navidad</t>
         </is>
       </c>
       <c r="F122" s="1" t="inlineStr">
@@ -4446,7 +4560,24 @@
           <t>der Gang</t>
         </is>
       </c>
-      <c r="C123" s="1" t="n"/>
+      <c r="C123" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Gänge.</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Gang in meiner Schule ist sehr weitläufig.</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El pasillo de mi escuela es muy amplio.</t>
+        </is>
+      </c>
       <c r="F123" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4470,6 +4601,12 @@
           <t>das Gedicht</t>
         </is>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El poema</t>
+        </is>
+      </c>
       <c r="F124" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4488,9 +4625,21 @@
 Die Ferien.</t>
         </is>
       </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Ferien.</t>
+        </is>
+      </c>
       <c r="D125" s="1" t="inlineStr">
         <is>
           <t>Der Urlaub</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist sehr interessant
+La vacación es muy interesante.</t>
         </is>
       </c>
       <c r="F125" s="1" t="inlineStr">
@@ -4511,9 +4660,21 @@
 Die Brief.</t>
         </is>
       </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Briefe.</t>
+        </is>
+      </c>
       <c r="D126" s="1" t="inlineStr">
         <is>
           <t>der Brief</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El carta.</t>
         </is>
       </c>
       <c r="F126" s="1" t="inlineStr">
@@ -4534,9 +4695,21 @@
 Die Stern.</t>
         </is>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Sterne.</t>
+        </is>
+      </c>
       <c r="D127" s="1" t="inlineStr">
         <is>
           <t>der Stern</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+el estrella</t>
         </is>
       </c>
       <c r="F127" s="1" t="inlineStr">
@@ -4557,9 +4730,21 @@
 Die Wurst.</t>
         </is>
       </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Würste.</t>
+        </is>
+      </c>
       <c r="D128" s="1" t="inlineStr">
         <is>
           <t>die Wurst</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La salchicha.</t>
         </is>
       </c>
       <c r="F128" s="1" t="inlineStr">
@@ -4579,7 +4764,24 @@
           <t>das Lieblingsfach</t>
         </is>
       </c>
-      <c r="C129" s="1" t="n"/>
+      <c r="C129" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Lieblingsfächer</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mein Lieblingsfach ist Deutsch.</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mi materia favorita es aleman.</t>
+        </is>
+      </c>
       <c r="F129" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4597,7 +4799,24 @@
           <t>die Note</t>
         </is>
       </c>
-      <c r="C130" s="1" t="n"/>
+      <c r="C130" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Noten</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich bin begeistert, dass ich die Note 1,0 erhalten habe.</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Estoy entusiasmado de haber recibido la calificación de 1.0.</t>
+        </is>
+      </c>
       <c r="F130" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4615,7 +4834,24 @@
           <t>die Geschichte</t>
         </is>
       </c>
-      <c r="C131" s="1" t="n"/>
+      <c r="C131" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Geschichten</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Geschichte hat uns viel zu erzählen.</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La historia tiene mucho que decirnos.</t>
+        </is>
+      </c>
       <c r="F131" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4637,6 +4873,12 @@
       <c r="D132" s="1" t="inlineStr">
         <is>
           <t>die Kunst</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La arte.</t>
         </is>
       </c>
       <c r="F132" s="1" t="inlineStr">

</xml_diff>

<commit_message>
this version improve the visual data in the terminal just using (*)
</commit_message>
<xml_diff>
--- a/Sustantivos_Aleman_Completo.xlsx
+++ b/Sustantivos_Aleman_Completo.xlsx
@@ -4110,7 +4110,12 @@
           <t>die Lösungen</t>
         </is>
       </c>
-      <c r="C110" s="1" t="n"/>
+      <c r="C110" s="1" t="inlineStr">
+        <is>
+          <t>,
+die Lösungen.</t>
+        </is>
+      </c>
       <c r="D110" t="inlineStr">
         <is>
           <t xml:space="preserve">
@@ -4596,6 +4601,12 @@
 Das Gedicht</t>
         </is>
       </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>:
+Die Gedichte</t>
+        </is>
+      </c>
       <c r="D124" s="1" t="inlineStr">
         <is>
           <t>das Gedicht</t>
@@ -4899,9 +4910,21 @@
 Angst</t>
         </is>
       </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Ängste</t>
+        </is>
+      </c>
       <c r="D133" s="1" t="inlineStr">
         <is>
           <t>die Angst</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La miedo</t>
         </is>
       </c>
       <c r="F133" s="1" t="inlineStr">
@@ -4921,7 +4944,24 @@
           <t>die Notenskala</t>
         </is>
       </c>
-      <c r="C134" s="1" t="n"/>
+      <c r="C134" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Notenskalen</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Notenskala reicht von 1 bis 6.</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La escala de calificación va de 1 a 6.</t>
+        </is>
+      </c>
       <c r="F134" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4940,9 +4980,21 @@
 Die Hausaufgabe</t>
         </is>
       </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Hausaufgaben mit ihrem Artikel.</t>
+        </is>
+      </c>
       <c r="D135" s="1" t="inlineStr">
         <is>
           <t>die Hausaufgabe</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La tarea.</t>
         </is>
       </c>
       <c r="F135" s="1" t="inlineStr">
@@ -4962,7 +5014,24 @@
           <t>die Prüfung</t>
         </is>
       </c>
-      <c r="C136" s="1" t="n"/>
+      <c r="C136" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Prüfungen</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich habe die Prüfung bestanden.</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+He pasado la prueba.</t>
+        </is>
+      </c>
       <c r="F136" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -4981,9 +5050,21 @@
 Die Fächer.</t>
         </is>
       </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Fächer.</t>
+        </is>
+      </c>
       <c r="D137" s="1" t="inlineStr">
         <is>
           <t>das Fach</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La materia.</t>
         </is>
       </c>
       <c r="F137" s="1" t="inlineStr">
@@ -5003,7 +5084,24 @@
           <t>der Landesmeister</t>
         </is>
       </c>
-      <c r="C138" s="1" t="n"/>
+      <c r="C138" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Landesmeister.</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der FC Bayern München hat vor kurzem zum vierten Mal in Folge den Titel des deutschen Landesmeisters errungen.</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El FC Bayern Munich ha ganado su cuarto título consecutivo del Campeonato Alemán recientemente.</t>
+        </is>
+      </c>
       <c r="F138" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5022,9 +5120,21 @@
 Die Pflichtschulbildung</t>
         </is>
       </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+Die Pflichtschulbildungen</t>
+        </is>
+      </c>
       <c r="D139" s="1" t="inlineStr">
         <is>
           <t>die Schulpflicht</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La Ley de la Educación Obligatoria.</t>
         </is>
       </c>
       <c r="F139" s="1" t="inlineStr">
@@ -5044,7 +5154,24 @@
           <t>die Dauer</t>
         </is>
       </c>
-      <c r="C140" s="1" t="n"/>
+      <c r="C140" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Dauern</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Dauer des Films war beeindruckend lang.</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La duración de la película fue impresionantemente larga.</t>
+        </is>
+      </c>
       <c r="F140" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5068,6 +5195,12 @@
           <t>die Satz</t>
         </is>
       </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La oración.</t>
+        </is>
+      </c>
       <c r="F141" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5086,6 +5219,18 @@
         </is>
       </c>
       <c r="C142" s="1" t="n"/>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich lerne gerne die Sätze meiner Muttersprache.</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Aprendo con gusto las frases de mi lengua materna.</t>
+        </is>
+      </c>
       <c r="F142" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5103,7 +5248,24 @@
           <t>der Lebenslauf</t>
         </is>
       </c>
-      <c r="C143" s="1" t="n"/>
+      <c r="C143" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Lebensläufe</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Lebenslauf bildet eine wichtige Voraussetzung bei Bewerbungen.</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El currículum es un requisito importante para las aplicaciones.</t>
+        </is>
+      </c>
       <c r="F143" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5121,7 +5283,24 @@
           <t>die Vorlesung</t>
         </is>
       </c>
-      <c r="C144" s="1" t="n"/>
+      <c r="C144" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Vorlesungen</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich habe die Vorlesung sehr genossen.</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Disfruté mucho de la clase.</t>
+        </is>
+      </c>
       <c r="F144" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5140,9 +5319,21 @@
 Der Stromkreis (elektrisch), Verbindung</t>
         </is>
       </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Stromkreise.</t>
+        </is>
+      </c>
       <c r="D145" s="1" t="inlineStr">
         <is>
           <t>die Schaltung</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La circuitería.</t>
         </is>
       </c>
       <c r="F145" s="1" t="inlineStr">
@@ -5163,9 +5354,22 @@
 Die Grundregel</t>
         </is>
       </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>, lautet: 
+Bei Nomen, die auf einen Konsonanten enden, fügt man an den Wortstamm ein "-s" an.
+Die Grundregeln mit ihren Artikeln lauten.</t>
+        </is>
+      </c>
       <c r="D146" s="1" t="inlineStr">
         <is>
           <t>die Grundregel</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La regla básica.</t>
         </is>
       </c>
       <c r="F146" s="1" t="inlineStr">
@@ -5185,7 +5389,24 @@
           <t>der Akzent</t>
         </is>
       </c>
-      <c r="C147" s="1" t="n"/>
+      <c r="C147" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Akzente.</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Akzent legt den Schwerpunkt auf die wichtigsten Wörter.</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El acento coloca el énfasis en las palabras más importantes.</t>
+        </is>
+      </c>
       <c r="F147" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5204,9 +5425,20 @@
 die Woche</t>
         </is>
       </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> fällt es ein: las semanas</t>
+        </is>
+      </c>
       <c r="D148" s="1" t="inlineStr">
         <is>
           <t>das Grundwort</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La palabra base.</t>
         </is>
       </c>
       <c r="F148" s="1" t="inlineStr">
@@ -5232,6 +5464,12 @@
           <t>der Stau</t>
         </is>
       </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+El atasco.</t>
+        </is>
+      </c>
       <c r="F149" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5250,9 +5488,21 @@
 Die Konferenz, Versammlung.</t>
         </is>
       </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Konferenzen, Versammlungen.</t>
+        </is>
+      </c>
       <c r="D150" s="1" t="inlineStr">
         <is>
           <t>die Besprechung</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> war nicht schön
+La reunión no fue agradable.</t>
         </is>
       </c>
       <c r="F150" s="1" t="inlineStr">
@@ -5273,9 +5523,21 @@
 Der Speisesaal</t>
         </is>
       </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>:
+Die Speisesäle</t>
+        </is>
+      </c>
       <c r="D151" s="1" t="inlineStr">
         <is>
           <t>die Kantine</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La cantina.</t>
         </is>
       </c>
       <c r="F151" s="1" t="inlineStr">
@@ -5296,9 +5558,21 @@
 Der Erwachsene</t>
         </is>
       </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Erwachsenen</t>
+        </is>
+      </c>
       <c r="D152" s="1" t="inlineStr">
         <is>
           <t>der Erwachsen</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>en
+Los adultos.</t>
         </is>
       </c>
       <c r="F152" s="1" t="inlineStr">
@@ -5318,7 +5592,24 @@
           <t>das Haupt</t>
         </is>
       </c>
-      <c r="C153" s="1" t="n"/>
+      <c r="C153" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Häupter</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Haupt ist ein wichtiger Bestandteil des menschlichen Körpers.</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La cabeza es una parte importante del cuerpo humano.</t>
+        </is>
+      </c>
       <c r="F153" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5337,9 +5628,21 @@
 Der Hauptcomputer</t>
         </is>
       </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> "der" ist ein maskulines Substantiv.
+ Computermachen.</t>
+        </is>
+      </c>
       <c r="D154" s="1" t="inlineStr">
         <is>
           <t>der Hauptrechner</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El servidor principal.</t>
         </is>
       </c>
       <c r="F154" s="1" t="inlineStr">
@@ -5359,7 +5662,24 @@
           <t>der Arbeitsbereich</t>
         </is>
       </c>
-      <c r="C155" s="1" t="n"/>
+      <c r="C155" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Arbeitsbereiche.</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+In meinem Arbeitsbereich ist ein sehr angenehmes Arbeitsumfeld entstanden.</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+En mi área de trabajo se ha creado un ambiente de trabajo muy agradable.</t>
+        </is>
+      </c>
       <c r="F155" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5378,9 +5698,21 @@
 Der Unternehmensarzt</t>
         </is>
       </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Unternehmensärzte mit ihren Artikeln</t>
+        </is>
+      </c>
       <c r="D156" s="1" t="inlineStr">
         <is>
           <t>der Betriebsarzt</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El médico de empresa.</t>
         </is>
       </c>
       <c r="F156" s="1" t="inlineStr">
@@ -5401,9 +5733,21 @@
 Die erste Kategorie.</t>
         </is>
       </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Das
+Die ersten Dinge.</t>
+        </is>
+      </c>
       <c r="D157" s="1" t="inlineStr">
         <is>
           <t>die Spitzenklasse</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+la clase de élite</t>
         </is>
       </c>
       <c r="F157" s="1" t="inlineStr">
@@ -5424,9 +5768,21 @@
 Das Büro.</t>
         </is>
       </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Büros.</t>
+        </is>
+      </c>
       <c r="D158" s="1" t="inlineStr">
         <is>
           <t>das Büro</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La oficina.</t>
         </is>
       </c>
       <c r="F158" s="1" t="inlineStr">
@@ -5452,6 +5808,12 @@
           <t>die Grundlage</t>
         </is>
       </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La base</t>
+        </is>
+      </c>
       <c r="F159" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5470,9 +5832,21 @@
 Der Aspekt.</t>
         </is>
       </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Aspekte.</t>
+        </is>
+      </c>
       <c r="D160" s="1" t="inlineStr">
         <is>
           <t>das Aussehen</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El aspecto</t>
         </is>
       </c>
       <c r="F160" s="1" t="inlineStr">
@@ -5493,9 +5867,21 @@
 Perspektiven für die Zukunft</t>
         </is>
       </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Perspektiven für die Zukunft</t>
+        </is>
+      </c>
       <c r="D161" s="1" t="inlineStr">
         <is>
           <t>die Zukunftsaussichten</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Las perspectivas de futuro</t>
         </is>
       </c>
       <c r="F161" s="1" t="inlineStr">
@@ -5521,6 +5907,12 @@
           <t>die Chance</t>
         </is>
       </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La oportunidad.</t>
+        </is>
+      </c>
       <c r="F162" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5539,9 +5931,21 @@
 Die Wirtschaft.</t>
         </is>
       </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Wirtschaften</t>
+        </is>
+      </c>
       <c r="D163" s="1" t="inlineStr">
         <is>
           <t>die Wirtschaft</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La economía.</t>
         </is>
       </c>
       <c r="F163" s="1" t="inlineStr">
@@ -5562,9 +5966,21 @@
 Die Gebühr</t>
         </is>
       </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Gebühren</t>
+        </is>
+      </c>
       <c r="D164" s="1" t="inlineStr">
         <is>
           <t>die Quote</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La cita.</t>
         </is>
       </c>
       <c r="F164" s="1" t="inlineStr">
@@ -5584,7 +6000,24 @@
           <t>die Möglichkeit</t>
         </is>
       </c>
-      <c r="C165" s="1" t="n"/>
+      <c r="C165" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Möglichkeiten</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Mit der richtigen Strategie eröffnet sich uns viele Möglichkeiten.</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+Con la estrategia correcta, nos abrirá muchas posibilidades.</t>
+        </is>
+      </c>
       <c r="F165" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5603,9 +6036,21 @@
 Die Nummer.</t>
         </is>
       </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Nummern.</t>
+        </is>
+      </c>
       <c r="D166" s="1" t="inlineStr">
         <is>
           <t>die Zahl</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist zwei
+La cifra es dos.</t>
         </is>
       </c>
       <c r="F166" s="1" t="inlineStr">
@@ -5625,7 +6070,24 @@
           <t>die Tendenz</t>
         </is>
       </c>
-      <c r="C167" s="1" t="n"/>
+      <c r="C167" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Tendenzen.</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Tendenz geht dahin, dass die Produktionskosten sinken.</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La tendencia es que los costos de producción disminuyan.</t>
+        </is>
+      </c>
       <c r="F167" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5644,9 +6106,21 @@
 der Universitätsabsolvent</t>
         </is>
       </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Universitätsabsolventen</t>
+        </is>
+      </c>
       <c r="D168" s="1" t="inlineStr">
         <is>
           <t>der Akademiker</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El académico.</t>
         </is>
       </c>
       <c r="F168" s="1" t="inlineStr">
@@ -5666,7 +6140,24 @@
           <t>der Betrieb</t>
         </is>
       </c>
-      <c r="C169" s="1" t="n"/>
+      <c r="C169" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Plural von der Betrieb ist die Betriebe.</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Betrieb hat seine Tore bereits heute morgen geöffnet.</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El negocio abrió sus puertas esta mañana temprano.</t>
+        </is>
+      </c>
       <c r="F169" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5685,9 +6176,21 @@
 Der Wirtschaftstechniker</t>
         </is>
       </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Wirtschaftstechniker mit ihren Artikeln.</t>
+        </is>
+      </c>
       <c r="D170" s="1" t="inlineStr">
         <is>
           <t>der Betriebswirt</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El administrador de negocios.</t>
         </is>
       </c>
       <c r="F170" s="1" t="inlineStr">
@@ -5707,7 +6210,24 @@
           <t>der Berufstätiger</t>
         </is>
       </c>
-      <c r="C171" s="1" t="n"/>
+      <c r="C171" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Berufstätigen.</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Berufstätige arbeitet viele Stunden pro Woche für seine Karriere.</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El trabajador dedica muchas horas a la semana a su carrera.</t>
+        </is>
+      </c>
       <c r="F171" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5725,7 +6245,24 @@
           <t>der Vertrag</t>
         </is>
       </c>
-      <c r="C172" s="1" t="n"/>
+      <c r="C172" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Verträge</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Vertrag muss noch unterzeichnet werden.</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El contrato debe firmarse aún.</t>
+        </is>
+      </c>
       <c r="F172" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5743,7 +6280,24 @@
           <t>die Probezeit</t>
         </is>
       </c>
-      <c r="C173" s="1" t="n"/>
+      <c r="C173" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Probezeiten</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich bin gerade am Ende meiner Probezeit.</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Estoy al final de mi periodo de prueba.</t>
+        </is>
+      </c>
       <c r="F173" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5761,7 +6315,24 @@
           <t>der Kauf</t>
         </is>
       </c>
-      <c r="C174" s="1" t="n"/>
+      <c r="C174" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Käufe.</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Kauf der neuen Software war eine gute Investition.</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La compra del nuevo software fue una buena inversión.</t>
+        </is>
+      </c>
       <c r="F174" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5780,9 +6351,21 @@
 Die Gesellschaft.</t>
         </is>
       </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Gesellschaften</t>
+        </is>
+      </c>
       <c r="D175" s="1" t="inlineStr">
         <is>
           <t>die Gesellschaft</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La sociedad.</t>
         </is>
       </c>
       <c r="F175" s="1" t="inlineStr">
@@ -5803,9 +6386,21 @@
 Der Entwicklung.</t>
         </is>
       </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Entwicklungen.</t>
+        </is>
+      </c>
       <c r="D176" s="1" t="inlineStr">
         <is>
           <t>die Entwicklung</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La evolución.</t>
         </is>
       </c>
       <c r="F176" s="1" t="inlineStr">
@@ -5826,9 +6421,21 @@
 Die Einstellung</t>
         </is>
       </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Einstellungen</t>
+        </is>
+      </c>
       <c r="D177" s="1" t="inlineStr">
         <is>
           <t>die Einstellung</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La actitud</t>
         </is>
       </c>
       <c r="F177" s="1" t="inlineStr">
@@ -5849,9 +6456,21 @@
 die Implementierung</t>
         </is>
       </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Implementierungen</t>
+        </is>
+      </c>
       <c r="D178" s="1" t="inlineStr">
         <is>
           <t>die Umsetzung</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La implementación</t>
         </is>
       </c>
       <c r="F178" s="1" t="inlineStr">
@@ -5872,9 +6491,21 @@
 Der Vertrag.</t>
         </is>
       </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Verträge.</t>
+        </is>
+      </c>
       <c r="D179" s="1" t="inlineStr">
         <is>
           <t>die Vereinbarung</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La convención.</t>
         </is>
       </c>
       <c r="F179" s="1" t="inlineStr">
@@ -5894,7 +6525,24 @@
           <t>der Einstieg</t>
         </is>
       </c>
-      <c r="C180" s="1" t="n"/>
+      <c r="C180" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Einstiege.</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Einstieg in das neue Jahr gestaltete sich schwierig.</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El comienzo del año nuevo fue difícil.</t>
+        </is>
+      </c>
       <c r="F180" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5913,9 +6561,21 @@
 Der Arbeitsbereich</t>
         </is>
       </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Arbeitsbereiche.</t>
+        </is>
+      </c>
       <c r="D181" s="1" t="inlineStr">
         <is>
           <t>der Arbeitsbereich</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El área de trabajo.</t>
         </is>
       </c>
       <c r="F181" s="1" t="inlineStr">
@@ -5935,7 +6595,24 @@
           <t>die Zulassung</t>
         </is>
       </c>
-      <c r="C182" s="1" t="n"/>
+      <c r="C182" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Zulassungen</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich muss meine Zulassung beim Straßenverkehrsamt verlängern.</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tengo que renovar mi licencia en la oficina de tráfico.</t>
+        </is>
+      </c>
       <c r="F182" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -5954,9 +6631,21 @@
 Die Garantie.</t>
         </is>
       </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Garantien.</t>
+        </is>
+      </c>
       <c r="D183" s="1" t="inlineStr">
         <is>
           <t>die Garantie</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+la garantía</t>
         </is>
       </c>
       <c r="F183" s="1" t="inlineStr">
@@ -5977,9 +6666,21 @@
 La palabra española es "significado" y la traducción al alemán es "Bedeutung".</t>
         </is>
       </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Bedeutungen</t>
+        </is>
+      </c>
       <c r="D184" s="1" t="inlineStr">
         <is>
           <t>die Bedeutung</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La significación.</t>
         </is>
       </c>
       <c r="F184" s="1" t="inlineStr">
@@ -5999,10 +6700,21 @@
           <t>die Wendung</t>
         </is>
       </c>
-      <c r="C185" s="1" t="n"/>
+      <c r="C185" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Wendungen</t>
+        </is>
+      </c>
       <c r="D185" s="1" t="inlineStr">
         <is>
           <t>sich zum Guten/Schlechten wenden</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Virar hacia el bien/mal.</t>
         </is>
       </c>
       <c r="F185" s="1" t="inlineStr">
@@ -6022,7 +6734,24 @@
           <t>der Jurist</t>
         </is>
       </c>
-      <c r="C186" s="1" t="n"/>
+      <c r="C186" s="1" t="inlineStr">
+        <is>
+          <t>:
+Die Juristen</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Jurist analysierte die relevanten Paragraphen des Gesetzes.</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El abogado analizó los artículos relevantes de la ley.</t>
+        </is>
+      </c>
       <c r="F186" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6040,7 +6769,24 @@
           <t>der Zahnarzt</t>
         </is>
       </c>
-      <c r="C187" s="1" t="n"/>
+      <c r="C187" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Zahnärzte</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Zahnarzt hat mich gestern untersucht.</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El dentista me examinó ayer.</t>
+        </is>
+      </c>
       <c r="F187" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6058,7 +6804,24 @@
           <t>die Welt</t>
         </is>
       </c>
-      <c r="C188" s="1" t="n"/>
+      <c r="C188" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Welten</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Welt ist ein faszinierender Ort voller Possibilitäten.</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El mundo es un lugar fascinante lleno de posibilidades.</t>
+        </is>
+      </c>
       <c r="F188" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6077,9 +6840,21 @@
 Apfelsaft</t>
         </is>
       </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Apfelsäfte</t>
+        </is>
+      </c>
       <c r="D189" s="1" t="inlineStr">
         <is>
           <t>der Apfelsaft</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El zumo de manzana.</t>
         </is>
       </c>
       <c r="F189" s="1" t="inlineStr">
@@ -6100,9 +6875,21 @@
 Das Flugzeug.</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Flugzeuge.</t>
+        </is>
+      </c>
       <c r="D190" s="1" t="inlineStr">
         <is>
           <t>das Flugzeug</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El avión.</t>
         </is>
       </c>
       <c r="F190" s="1" t="inlineStr">
@@ -6128,6 +6915,12 @@
           <t>die Form</t>
         </is>
       </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La forma</t>
+        </is>
+      </c>
       <c r="F191" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6146,9 +6939,21 @@
 Die Neugier.</t>
         </is>
       </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Neugierden.</t>
+        </is>
+      </c>
       <c r="D192" s="1" t="inlineStr">
         <is>
           <t>die Sehenswürdigkeiten</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Las atracciones turísticas.</t>
         </is>
       </c>
       <c r="F192" s="1" t="inlineStr">
@@ -6169,9 +6974,21 @@
 Das Gerät.</t>
         </is>
       </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Geräte.</t>
+        </is>
+      </c>
       <c r="D193" s="1" t="inlineStr">
         <is>
           <t>der Apparat</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El aparato.</t>
         </is>
       </c>
       <c r="F193" s="1" t="inlineStr">
@@ -6192,9 +7009,21 @@
 Der Sonne</t>
         </is>
       </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Sonnen</t>
+        </is>
+      </c>
       <c r="D194" s="1" t="inlineStr">
         <is>
           <t>die Sonne</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist schön
+La sol es hermosa.</t>
         </is>
       </c>
       <c r="F194" s="1" t="inlineStr">
@@ -6215,9 +7044,21 @@
 Der Weg, nach draußen.</t>
         </is>
       </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Wege, nach draußen.</t>
+        </is>
+      </c>
       <c r="D195" s="1" t="inlineStr">
         <is>
           <t>der Weg</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El camino.</t>
         </is>
       </c>
       <c r="F195" s="1" t="inlineStr">
@@ -6238,9 +7079,21 @@
 Die Brille.</t>
         </is>
       </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Brillen.</t>
+        </is>
+      </c>
       <c r="D196" s="1" t="inlineStr">
         <is>
           <t>die Brille</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La gafa.</t>
         </is>
       </c>
       <c r="F196" s="1" t="inlineStr">
@@ -6260,7 +7113,24 @@
           <t>der Satzbau</t>
         </is>
       </c>
-      <c r="C197" s="1" t="n"/>
+      <c r="C197" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Satzbäume.</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Satzbau ist eine Grundlage der deutschen Grammatik.</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La estructura de la frase es una base para la gramática alemana.</t>
+        </is>
+      </c>
       <c r="F197" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6279,9 +7149,21 @@
 Das Verb</t>
         </is>
       </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Dasen</t>
+        </is>
+      </c>
       <c r="D198" s="1" t="inlineStr">
         <is>
           <t>das Verb</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+el verbo</t>
         </is>
       </c>
       <c r="F198" s="1" t="inlineStr">
@@ -6302,9 +7184,21 @@
 Der Präfix</t>
         </is>
       </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>:
+Die Präfixe</t>
+        </is>
+      </c>
       <c r="D199" s="1" t="inlineStr">
         <is>
           <t>das Präfix</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+el prefijo</t>
         </is>
       </c>
       <c r="F199" s="1" t="inlineStr">
@@ -6324,7 +7218,24 @@
           <t>das Wort</t>
         </is>
       </c>
-      <c r="C200" s="1" t="n"/>
+      <c r="C200" s="1" t="inlineStr">
+        <is>
+          <t>:
+die Wörter</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Das Wort kann viele verschiedene Bedeutungen haben.</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La palabra puede tener muchos significados diferentes.</t>
+        </is>
+      </c>
       <c r="F200" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6342,7 +7253,24 @@
           <t>der Regenschirm</t>
         </is>
       </c>
-      <c r="C201" s="1" t="n"/>
+      <c r="C201" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Regenschirme.</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Regenschirm schützt mich vor dem Regen.</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El paraguas me protege del lluvia.</t>
+        </is>
+      </c>
       <c r="F201" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6361,9 +7289,21 @@
 Der Himmel.</t>
         </is>
       </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Himmel.</t>
+        </is>
+      </c>
       <c r="D202" s="1" t="inlineStr">
         <is>
           <t>der Himmel</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist blau
+El cielo es azul.</t>
         </is>
       </c>
       <c r="F202" s="1" t="inlineStr">
@@ -6389,6 +7329,12 @@
           <t>die Vorstellung</t>
         </is>
       </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+la presentación</t>
+        </is>
+      </c>
       <c r="F203" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6407,9 +7353,21 @@
 Der Montierer.</t>
         </is>
       </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Montierer.</t>
+        </is>
+      </c>
       <c r="D204" s="1" t="inlineStr">
         <is>
           <t>der Monteur</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El mecánico.</t>
         </is>
       </c>
       <c r="F204" s="1" t="inlineStr">
@@ -6429,7 +7387,24 @@
           <t>der Knoblauch</t>
         </is>
       </c>
-      <c r="C205" s="1" t="n"/>
+      <c r="C205" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Knoblauchzehen.</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Knoblauchtee war eine Wohltat für meine reizende Kehle.</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El té de ajo fue un bálsamo para mi dulce garganta.</t>
+        </is>
+      </c>
       <c r="F205" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6448,9 +7423,21 @@
 Die Film.</t>
         </is>
       </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Filme.</t>
+        </is>
+      </c>
       <c r="D206" s="1" t="inlineStr">
         <is>
           <t>der Film</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist aus
+La película ha terminado.</t>
         </is>
       </c>
       <c r="F206" s="1" t="inlineStr">
@@ -6470,7 +7457,24 @@
           <t>das Taxi</t>
         </is>
       </c>
-      <c r="C207" s="1" t="n"/>
+      <c r="C207" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Taxis.</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich musste meine Pläne ändern und stattdessen ein Taxi nehmen.</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Tuve que cambiar mis planes y tomar un taxi en lugar de eso.</t>
+        </is>
+      </c>
       <c r="F207" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6488,7 +7492,24 @@
           <t>der Gast</t>
         </is>
       </c>
-      <c r="C208" s="1" t="n"/>
+      <c r="C208" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Gäste</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Der Gast war sehr zufrieden mit dem Abendessen.</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El invitado estaba muy satisfecho con la cena.</t>
+        </is>
+      </c>
       <c r="F208" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6507,9 +7528,21 @@
 Die Gäste</t>
         </is>
       </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Gäste.</t>
+        </is>
+      </c>
       <c r="D209" s="1" t="inlineStr">
         <is>
           <t>die Gäste</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Los invitados.</t>
         </is>
       </c>
       <c r="F209" s="1" t="inlineStr">
@@ -6530,9 +7563,21 @@
 Die Empfindung</t>
         </is>
       </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Empfindungen</t>
+        </is>
+      </c>
       <c r="D210" s="1" t="inlineStr">
         <is>
           <t>das Aufsehen</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El revuelo</t>
         </is>
       </c>
       <c r="F210" s="1" t="inlineStr">
@@ -6553,9 +7598,21 @@
 Die Wissenschaft.</t>
         </is>
       </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Wissenschaften.</t>
+        </is>
+      </c>
       <c r="D211" s="1" t="inlineStr">
         <is>
           <t>die Wissenschaft</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+la ciencia</t>
         </is>
       </c>
       <c r="F211" s="1" t="inlineStr">
@@ -6576,9 +7633,21 @@
 Die Lage.</t>
         </is>
       </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Lagen.</t>
+        </is>
+      </c>
       <c r="D212" s="1" t="inlineStr">
         <is>
           <t>die Lokalisierung</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La localización.</t>
         </is>
       </c>
       <c r="F212" s="1" t="inlineStr">
@@ -6599,9 +7668,21 @@
 Die Beteiligung</t>
         </is>
       </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Beteiligungen.</t>
+        </is>
+      </c>
       <c r="D213" s="1" t="inlineStr">
         <is>
           <t>die Beteiligung</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La participación</t>
         </is>
       </c>
       <c r="F213" s="1" t="inlineStr">
@@ -6622,9 +7703,21 @@
 Der Sektor.</t>
         </is>
       </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Sektoren</t>
+        </is>
+      </c>
       <c r="D214" s="1" t="inlineStr">
         <is>
           <t>die Branche</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La industria.</t>
         </is>
       </c>
       <c r="F214" s="1" t="inlineStr">
@@ -6645,9 +7738,21 @@
 Der Stoß</t>
         </is>
       </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Stöße</t>
+        </is>
+      </c>
       <c r="D215" s="1" t="inlineStr">
         <is>
           <t>der Schub</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>kasten
+el cajón de almacenamiento</t>
         </is>
       </c>
       <c r="F215" s="1" t="inlineStr">
@@ -6673,6 +7778,12 @@
           <t>das Paket</t>
         </is>
       </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ist hier
+El paquete está aquí.</t>
+        </is>
+      </c>
       <c r="F216" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6690,7 +7801,24 @@
           <t>das Instrument</t>
         </is>
       </c>
-      <c r="C217" s="1" t="n"/>
+      <c r="C217" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+die Instrumente</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Ich lerne gerne neue Instrumente kennen.</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Me gusta conocer nuevos instrumentos.</t>
+        </is>
+      </c>
       <c r="F217" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6714,6 +7842,12 @@
           <t>das Garten</t>
         </is>
       </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>haus
+La casa de jardín.</t>
+        </is>
+      </c>
       <c r="F218" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6737,6 +7871,12 @@
           <t>der Vorschlag</t>
         </is>
       </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+La propuesta</t>
+        </is>
+      </c>
       <c r="F219" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6760,6 +7900,12 @@
           <t>das Internet</t>
         </is>
       </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+El internet.</t>
+        </is>
+      </c>
       <c r="F220" s="1" t="inlineStr">
         <is>
           <t>sustantivo</t>
@@ -6778,9 +7924,21 @@
 Der Konzert</t>
         </is>
       </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Die Konzertmitglieder</t>
+        </is>
+      </c>
       <c r="D221" s="1" t="inlineStr">
         <is>
           <t>das Konzert</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> beginnt um 8 Uhr
+El concierto comienza a las 8.</t>
         </is>
       </c>
       <c r="F221" s="1" t="inlineStr">

</xml_diff>